<commit_message>
feat: Enhance AI agent with SQL database integration and logging; add new API routes for AI interactions
</commit_message>
<xml_diff>
--- a/static/small.xlsx
+++ b/static/small.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Project Role</t>
   </si>
@@ -53,27 +53,12 @@
     <t>Ghosh</t>
   </si>
   <si>
-    <t>Gomkale</t>
-  </si>
-  <si>
     <t>Email ID</t>
   </si>
   <si>
-    <t>Backend Developer</t>
-  </si>
-  <si>
     <t>Fullstack Developer</t>
   </si>
   <si>
-    <t>Frontend Developer</t>
-  </si>
-  <si>
-    <t>Angular</t>
-  </si>
-  <si>
-    <t>Docker, SQL, Angular</t>
-  </si>
-  <si>
     <t>asdasdasd@temp.com</t>
   </si>
   <si>
@@ -83,23 +68,32 @@
     <t>tertertert@temp.com</t>
   </si>
   <si>
-    <t>Ahhh</t>
-  </si>
-  <si>
-    <t>VBggg</t>
-  </si>
-  <si>
-    <t>Njjjsdfjsdf</t>
-  </si>
-  <si>
-    <t>Viksdfdsf</t>
+    <t>Ashu</t>
+  </si>
+  <si>
+    <t>Das</t>
+  </si>
+  <si>
+    <t>Nilesh</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Tripathi</t>
+  </si>
+  <si>
+    <t>.Net, SQL, Angular</t>
+  </si>
+  <si>
+    <t>Angular, React</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +108,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -143,12 +143,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -477,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -498,7 +501,7 @@
     <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.625" customWidth="1"/>
     <col min="5" max="5" width="29.75" customWidth="1"/>
-    <col min="6" max="6" width="20.125" customWidth="1"/>
+    <col min="6" max="6" width="32.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -512,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -521,65 +524,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2">
-        <v>23423</v>
+        <v>458789</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3">
+        <v>589698</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2344234</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
+      <c r="A4">
+        <v>215468</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>423434</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
+    <row r="5" spans="1:6">
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F107"/>
@@ -595,6 +603,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Contributor xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9">
+      <UserInfo xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9">
+        <DisplayName xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
+        <AccountId xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xsi:nil="true"/>
+        <AccountType xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
+      </UserInfo>
+    </Contributor>
+    <CurrentStatus xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xsi:nil="true"/>
+    <BriefDescription xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xsi:nil="true"/>
+    <TaxCatchAll xmlns="3c35e321-f73a-4dae-ae38-a0459de24735" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004474A0DB76EA7E42929A3358CE3D3805" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e6c93514f1bce30700f46fe02e6806c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xmlns:ns3="ff8c5244-5f7b-46ae-80f1-1a8f4130f88b" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dfd0452339067cad8ebf177fe06a357" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
@@ -890,36 +927,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE49E316-C69F-4FCD-ABC4-9D0D1DF75F8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3c35e321-f73a-4dae-ae38-a0459de24735"/>
+    <ds:schemaRef ds:uri="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff8c5244-5f7b-46ae-80f1-1a8f4130f88b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Contributor xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9">
-      <UserInfo xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9">
-        <DisplayName xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
-        <AccountId xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xsi:nil="true"/>
-        <AccountType xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
-      </UserInfo>
-    </Contributor>
-    <CurrentStatus xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xsi:nil="true"/>
-    <BriefDescription xmlns="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9" xsi:nil="true"/>
-    <TaxCatchAll xmlns="3c35e321-f73a-4dae-ae38-a0459de24735" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FE2056D-CE60-4231-8AD4-A92B41BB6233}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F35AD7A2-E74A-497B-8864-CD9A252491F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -937,30 +971,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FE2056D-CE60-4231-8AD4-A92B41BB6233}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE49E316-C69F-4FCD-ABC4-9D0D1DF75F8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3c35e321-f73a-4dae-ae38-a0459de24735"/>
-    <ds:schemaRef ds:uri="c0f20f50-59cd-49ef-bdbb-aaf66b93f2c9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff8c5244-5f7b-46ae-80f1-1a8f4130f88b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>